<commit_message>
corregir indice de marco acumulativo
</commit_message>
<xml_diff>
--- a/data/Marco acumulativo.xlsx
+++ b/data/Marco acumulativo.xlsx
@@ -456,7 +456,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -536,7 +536,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" t="n">
         <v>13</v>
       </c>
       <c r="B12" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="A13" t="n">
         <v>15</v>
       </c>
       <c r="B13" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
+      <c r="A14" t="n">
         <v>19</v>
       </c>
       <c r="B14" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
+      <c r="A15" t="n">
         <v>20</v>
       </c>
       <c r="B15" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
+      <c r="A16" t="n">
         <v>21</v>
       </c>
       <c r="B16" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
+      <c r="A17" t="n">
         <v>23</v>
       </c>
       <c r="B17" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
+      <c r="A18" t="n">
         <v>26</v>
       </c>
       <c r="B18" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
+      <c r="A19" t="n">
         <v>27</v>
       </c>
       <c r="B19" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
+      <c r="A20" t="n">
         <v>28</v>
       </c>
       <c r="B20" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
+      <c r="A21" t="n">
         <v>32</v>
       </c>
       <c r="B21" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
+      <c r="A22" t="n">
         <v>35</v>
       </c>
       <c r="B22" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
+      <c r="A23" t="n">
         <v>44</v>
       </c>
       <c r="B23" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
+      <c r="A24" t="n">
         <v>45</v>
       </c>
       <c r="B24" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
+      <c r="A25" t="n">
         <v>49</v>
       </c>
       <c r="B25" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
+      <c r="A26" t="n">
         <v>50</v>
       </c>
       <c r="B26" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
+      <c r="A27" t="n">
         <v>51</v>
       </c>
       <c r="B27" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
+      <c r="A28" t="n">
         <v>52</v>
       </c>
       <c r="B28" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
+      <c r="A29" t="n">
         <v>53</v>
       </c>
       <c r="B29" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
+      <c r="A30" t="n">
         <v>54</v>
       </c>
       <c r="B30" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
+      <c r="A31" t="n">
         <v>55</v>
       </c>
       <c r="B31" t="inlineStr">
@@ -1056,7 +1056,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
+      <c r="A32" t="n">
         <v>56</v>
       </c>
       <c r="B32" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
+      <c r="A33" t="n">
         <v>57</v>
       </c>
       <c r="B33" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
+      <c r="A34" t="n">
         <v>58</v>
       </c>
       <c r="B34" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
+      <c r="A35" t="n">
         <v>59</v>
       </c>
       <c r="B35" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
+      <c r="A36" t="n">
         <v>61</v>
       </c>
       <c r="B36" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
+      <c r="A37" t="n">
         <v>62</v>
       </c>
       <c r="B37" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
+      <c r="A38" t="n">
         <v>63</v>
       </c>
       <c r="B38" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
+      <c r="A39" t="n">
         <v>64</v>
       </c>
       <c r="B39" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
+      <c r="A40" t="n">
         <v>66</v>
       </c>
       <c r="B40" t="inlineStr">
@@ -1236,7 +1236,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
+      <c r="A41" t="n">
         <v>67</v>
       </c>
       <c r="B41" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
+      <c r="A42" t="n">
         <v>68</v>
       </c>
       <c r="B42" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
+      <c r="A43" t="n">
         <v>69</v>
       </c>
       <c r="B43" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
+      <c r="A44" t="n">
         <v>70</v>
       </c>
       <c r="B44" t="inlineStr">
@@ -1316,7 +1316,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
+      <c r="A45" t="n">
         <v>71</v>
       </c>
       <c r="B45" t="inlineStr">
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
+      <c r="A46" t="n">
         <v>72</v>
       </c>
       <c r="B46" t="inlineStr">
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
+      <c r="A47" t="n">
         <v>73</v>
       </c>
       <c r="B47" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
+      <c r="A48" t="n">
         <v>74</v>
       </c>
       <c r="B48" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
+      <c r="A49" t="n">
         <v>75</v>
       </c>
       <c r="B49" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
+      <c r="A50" t="n">
         <v>76</v>
       </c>
       <c r="B50" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
+      <c r="A51" t="n">
         <v>77</v>
       </c>
       <c r="B51" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
+      <c r="A52" t="n">
         <v>88</v>
       </c>
       <c r="B52" t="inlineStr">
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
+      <c r="A53" t="n">
         <v>89</v>
       </c>
       <c r="B53" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
+      <c r="A54" t="n">
         <v>90</v>
       </c>
       <c r="B54" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
+      <c r="A55" t="n">
         <v>92</v>
       </c>
       <c r="B55" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
+      <c r="A56" t="n">
         <v>93</v>
       </c>
       <c r="B56" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
+      <c r="A57" t="n">
         <v>94</v>
       </c>
       <c r="B57" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
+      <c r="A58" t="n">
         <v>95</v>
       </c>
       <c r="B58" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
+      <c r="A59" t="n">
         <v>96</v>
       </c>
       <c r="B59" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
+      <c r="A60" t="n">
         <v>97</v>
       </c>
       <c r="B60" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
+      <c r="A61" t="n">
         <v>98</v>
       </c>
       <c r="B61" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
+      <c r="A62" t="n">
         <v>106</v>
       </c>
       <c r="B62" t="inlineStr">
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
+      <c r="A63" t="n">
         <v>107</v>
       </c>
       <c r="B63" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
+      <c r="A64" t="n">
         <v>108</v>
       </c>
       <c r="B64" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
+      <c r="A65" t="n">
         <v>109</v>
       </c>
       <c r="B65" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
+      <c r="A66" t="n">
         <v>110</v>
       </c>
       <c r="B66" t="inlineStr">
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
+      <c r="A67" t="n">
         <v>111</v>
       </c>
       <c r="B67" t="inlineStr">
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
+      <c r="A68" t="n">
         <v>112</v>
       </c>
       <c r="B68" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
+      <c r="A69" t="n">
         <v>114</v>
       </c>
       <c r="B69" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
+      <c r="A70" t="n">
         <v>115</v>
       </c>
       <c r="B70" t="inlineStr">
@@ -1836,7 +1836,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
+      <c r="A71" t="n">
         <v>116</v>
       </c>
       <c r="B71" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
+      <c r="A72" t="n">
         <v>117</v>
       </c>
       <c r="B72" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
+      <c r="A73" t="n">
         <v>118</v>
       </c>
       <c r="B73" t="inlineStr">
@@ -1896,7 +1896,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
+      <c r="A74" t="n">
         <v>119</v>
       </c>
       <c r="B74" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
+      <c r="A75" t="n">
         <v>121</v>
       </c>
       <c r="B75" t="inlineStr">
@@ -1936,7 +1936,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
+      <c r="A76" t="n">
         <v>122</v>
       </c>
       <c r="B76" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
+      <c r="A77" t="n">
         <v>123</v>
       </c>
       <c r="B77" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
+      <c r="A78" t="n">
         <v>129</v>
       </c>
       <c r="B78" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
+      <c r="A79" t="n">
         <v>130</v>
       </c>
       <c r="B79" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
+      <c r="A80" t="n">
         <v>131</v>
       </c>
       <c r="B80" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
+      <c r="A81" t="n">
         <v>132</v>
       </c>
       <c r="B81" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
+      <c r="A82" t="n">
         <v>138</v>
       </c>
       <c r="B82" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
+      <c r="A83" t="n">
         <v>162</v>
       </c>
       <c r="B83" t="inlineStr">
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
+      <c r="A84" t="n">
         <v>163</v>
       </c>
       <c r="B84" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
+      <c r="A85" t="n">
         <v>164</v>
       </c>
       <c r="B85" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
+      <c r="A86" t="n">
         <v>165</v>
       </c>
       <c r="B86" t="inlineStr">
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
+      <c r="A87" t="n">
         <v>166</v>
       </c>
       <c r="B87" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
+      <c r="A88" t="n">
         <v>167</v>
       </c>
       <c r="B88" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
+      <c r="A89" t="n">
         <v>168</v>
       </c>
       <c r="B89" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
+      <c r="A90" t="n">
         <v>176</v>
       </c>
       <c r="B90" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
+      <c r="A91" t="n">
         <v>177</v>
       </c>
       <c r="B91" t="inlineStr">
@@ -2256,7 +2256,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
+      <c r="A92" t="n">
         <v>178</v>
       </c>
       <c r="B92" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
+      <c r="A93" t="n">
         <v>179</v>
       </c>
       <c r="B93" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
+      <c r="A94" t="n">
         <v>180</v>
       </c>
       <c r="B94" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
+      <c r="A95" t="n">
         <v>181</v>
       </c>
       <c r="B95" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
+      <c r="A96" t="n">
         <v>182</v>
       </c>
       <c r="B96" t="inlineStr">
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
+      <c r="A97" t="n">
         <v>183</v>
       </c>
       <c r="B97" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
+      <c r="A98" t="n">
         <v>184</v>
       </c>
       <c r="B98" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
+      <c r="A99" t="n">
         <v>185</v>
       </c>
       <c r="B99" t="inlineStr">
@@ -2416,7 +2416,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
+      <c r="A100" t="n">
         <v>186</v>
       </c>
       <c r="B100" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
+      <c r="A101" t="n">
         <v>187</v>
       </c>
       <c r="B101" t="inlineStr">
@@ -2456,7 +2456,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
+      <c r="A102" t="n">
         <v>188</v>
       </c>
       <c r="B102" t="inlineStr">
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
+      <c r="A103" t="n">
         <v>189</v>
       </c>
       <c r="B103" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
+      <c r="A104" t="n">
         <v>213</v>
       </c>
       <c r="B104" t="inlineStr">
@@ -2516,7 +2516,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
+      <c r="A105" t="n">
         <v>218</v>
       </c>
       <c r="B105" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
+      <c r="A106" t="n">
         <v>221</v>
       </c>
       <c r="B106" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
+      <c r="A107" t="n">
         <v>222</v>
       </c>
       <c r="B107" t="inlineStr">
@@ -2576,7 +2576,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
+      <c r="A108" t="n">
         <v>224</v>
       </c>
       <c r="B108" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
+      <c r="A109" t="n">
         <v>225</v>
       </c>
       <c r="B109" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
+      <c r="A110" t="n">
         <v>226</v>
       </c>
       <c r="B110" t="inlineStr">
@@ -2636,7 +2636,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
+      <c r="A111" t="n">
         <v>227</v>
       </c>
       <c r="B111" t="inlineStr">
@@ -2656,7 +2656,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
+      <c r="A112" t="n">
         <v>228</v>
       </c>
       <c r="B112" t="inlineStr">
@@ -2676,7 +2676,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
+      <c r="A113" t="n">
         <v>229</v>
       </c>
       <c r="B113" t="inlineStr">
@@ -2696,7 +2696,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
+      <c r="A114" t="n">
         <v>230</v>
       </c>
       <c r="B114" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
+      <c r="A115" t="n">
         <v>231</v>
       </c>
       <c r="B115" t="inlineStr">
@@ -2736,7 +2736,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
+      <c r="A116" t="n">
         <v>235</v>
       </c>
       <c r="B116" t="inlineStr">
@@ -2756,7 +2756,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
+      <c r="A117" t="n">
         <v>237</v>
       </c>
       <c r="B117" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
+      <c r="A118" t="n">
         <v>238</v>
       </c>
       <c r="B118" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
+      <c r="A119" t="n">
         <v>239</v>
       </c>
       <c r="B119" t="inlineStr">
@@ -2816,7 +2816,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
+      <c r="A120" t="n">
         <v>240</v>
       </c>
       <c r="B120" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
+      <c r="A121" t="n">
         <v>241</v>
       </c>
       <c r="B121" t="inlineStr">
@@ -2856,7 +2856,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
+      <c r="A122" t="n">
         <v>243</v>
       </c>
       <c r="B122" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
+      <c r="A123" t="n">
         <v>249</v>
       </c>
       <c r="B123" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
+      <c r="A124" t="n">
         <v>250</v>
       </c>
       <c r="B124" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
+      <c r="A125" t="n">
         <v>251</v>
       </c>
       <c r="B125" t="inlineStr">
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n">
+      <c r="A126" t="n">
         <v>252</v>
       </c>
       <c r="B126" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n">
+      <c r="A127" t="n">
         <v>1</v>
       </c>
       <c r="B127" t="inlineStr">
@@ -2976,7 +2976,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
+      <c r="A128" t="n">
         <v>10</v>
       </c>
       <c r="B128" t="inlineStr">
@@ -2996,7 +2996,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n">
+      <c r="A129" t="n">
         <v>36</v>
       </c>
       <c r="B129" t="inlineStr">
@@ -3016,7 +3016,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n">
+      <c r="A130" t="n">
         <v>41</v>
       </c>
       <c r="B130" t="inlineStr">
@@ -3036,7 +3036,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n">
+      <c r="A131" t="n">
         <v>42</v>
       </c>
       <c r="B131" t="inlineStr">
@@ -3056,7 +3056,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
+      <c r="A132" t="n">
         <v>43</v>
       </c>
       <c r="B132" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n">
+      <c r="A133" t="n">
         <v>46</v>
       </c>
       <c r="B133" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n">
+      <c r="A134" t="n">
         <v>48</v>
       </c>
       <c r="B134" t="inlineStr">
@@ -3116,7 +3116,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n">
+      <c r="A135" t="n">
         <v>65</v>
       </c>
       <c r="B135" t="inlineStr">
@@ -3136,7 +3136,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n">
+      <c r="A136" t="n">
         <v>133</v>
       </c>
       <c r="B136" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n">
+      <c r="A137" t="n">
         <v>148</v>
       </c>
       <c r="B137" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n">
+      <c r="A138" t="n">
         <v>149</v>
       </c>
       <c r="B138" t="inlineStr">
@@ -3196,7 +3196,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="n">
+      <c r="A139" t="n">
         <v>150</v>
       </c>
       <c r="B139" t="inlineStr">
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="n">
+      <c r="A140" t="n">
         <v>151</v>
       </c>
       <c r="B140" t="inlineStr">
@@ -3236,7 +3236,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n">
+      <c r="A141" t="n">
         <v>152</v>
       </c>
       <c r="B141" t="inlineStr">
@@ -3256,7 +3256,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n">
+      <c r="A142" t="n">
         <v>155</v>
       </c>
       <c r="B142" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n">
+      <c r="A143" t="n">
         <v>161</v>
       </c>
       <c r="B143" t="inlineStr">
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n">
+      <c r="A144" t="n">
         <v>203</v>
       </c>
       <c r="B144" t="inlineStr">
@@ -3316,7 +3316,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
+      <c r="A145" t="n">
         <v>206</v>
       </c>
       <c r="B145" t="inlineStr">
@@ -3336,7 +3336,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="n">
+      <c r="A146" t="n">
         <v>211</v>
       </c>
       <c r="B146" t="inlineStr">
@@ -3356,7 +3356,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="1" t="n">
+      <c r="A147" t="n">
         <v>214</v>
       </c>
       <c r="B147" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="1" t="n">
+      <c r="A148" t="n">
         <v>216</v>
       </c>
       <c r="B148" t="inlineStr">
@@ -3396,7 +3396,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="1" t="n">
+      <c r="A149" t="n">
         <v>217</v>
       </c>
       <c r="B149" t="inlineStr">
@@ -3416,7 +3416,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="n">
+      <c r="A150" t="n">
         <v>14</v>
       </c>
       <c r="B150" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="1" t="n">
+      <c r="A151" t="n">
         <v>16</v>
       </c>
       <c r="B151" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="n">
+      <c r="A152" t="n">
         <v>17</v>
       </c>
       <c r="B152" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="n">
+      <c r="A153" t="n">
         <v>18</v>
       </c>
       <c r="B153" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="1" t="n">
+      <c r="A154" t="n">
         <v>22</v>
       </c>
       <c r="B154" t="inlineStr">
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="1" t="n">
+      <c r="A155" t="n">
         <v>24</v>
       </c>
       <c r="B155" t="inlineStr">
@@ -3536,7 +3536,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="1" t="n">
+      <c r="A156" t="n">
         <v>25</v>
       </c>
       <c r="B156" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="1" t="n">
+      <c r="A157" t="n">
         <v>29</v>
       </c>
       <c r="B157" t="inlineStr">
@@ -3576,7 +3576,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="n">
+      <c r="A158" t="n">
         <v>30</v>
       </c>
       <c r="B158" t="inlineStr">
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="1" t="n">
+      <c r="A159" t="n">
         <v>31</v>
       </c>
       <c r="B159" t="inlineStr">
@@ -3616,7 +3616,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="1" t="n">
+      <c r="A160" t="n">
         <v>33</v>
       </c>
       <c r="B160" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="1" t="n">
+      <c r="A161" t="n">
         <v>34</v>
       </c>
       <c r="B161" t="inlineStr">
@@ -3656,7 +3656,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="1" t="n">
+      <c r="A162" t="n">
         <v>38</v>
       </c>
       <c r="B162" t="inlineStr">
@@ -3676,7 +3676,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="1" t="n">
+      <c r="A163" t="n">
         <v>40</v>
       </c>
       <c r="B163" t="inlineStr">
@@ -3696,7 +3696,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="1" t="n">
+      <c r="A164" t="n">
         <v>79</v>
       </c>
       <c r="B164" t="inlineStr">
@@ -3716,7 +3716,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="1" t="n">
+      <c r="A165" t="n">
         <v>80</v>
       </c>
       <c r="B165" t="inlineStr">
@@ -3736,7 +3736,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="1" t="n">
+      <c r="A166" t="n">
         <v>82</v>
       </c>
       <c r="B166" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="n">
+      <c r="A167" t="n">
         <v>83</v>
       </c>
       <c r="B167" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="1" t="n">
+      <c r="A168" t="n">
         <v>99</v>
       </c>
       <c r="B168" t="inlineStr">
@@ -3796,7 +3796,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="1" t="n">
+      <c r="A169" t="n">
         <v>100</v>
       </c>
       <c r="B169" t="inlineStr">
@@ -3816,7 +3816,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="1" t="n">
+      <c r="A170" t="n">
         <v>102</v>
       </c>
       <c r="B170" t="inlineStr">
@@ -3836,7 +3836,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="1" t="n">
+      <c r="A171" t="n">
         <v>103</v>
       </c>
       <c r="B171" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="1" t="n">
+      <c r="A172" t="n">
         <v>128</v>
       </c>
       <c r="B172" t="inlineStr">
@@ -3876,7 +3876,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="1" t="n">
+      <c r="A173" t="n">
         <v>153</v>
       </c>
       <c r="B173" t="inlineStr">
@@ -3896,7 +3896,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="1" t="n">
+      <c r="A174" t="n">
         <v>169</v>
       </c>
       <c r="B174" t="inlineStr">
@@ -3916,7 +3916,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="1" t="n">
+      <c r="A175" t="n">
         <v>170</v>
       </c>
       <c r="B175" t="inlineStr">
@@ -3936,7 +3936,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="1" t="n">
+      <c r="A176" t="n">
         <v>171</v>
       </c>
       <c r="B176" t="inlineStr">
@@ -3956,7 +3956,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="1" t="n">
+      <c r="A177" t="n">
         <v>172</v>
       </c>
       <c r="B177" t="inlineStr">
@@ -3976,7 +3976,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="1" t="n">
+      <c r="A178" t="n">
         <v>173</v>
       </c>
       <c r="B178" t="inlineStr">
@@ -3996,7 +3996,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="1" t="n">
+      <c r="A179" t="n">
         <v>175</v>
       </c>
       <c r="B179" t="inlineStr">
@@ -4016,7 +4016,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="1" t="n">
+      <c r="A180" t="n">
         <v>204</v>
       </c>
       <c r="B180" t="inlineStr">
@@ -4036,7 +4036,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="1" t="n">
+      <c r="A181" t="n">
         <v>208</v>
       </c>
       <c r="B181" t="inlineStr">
@@ -4056,7 +4056,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="1" t="n">
+      <c r="A182" t="n">
         <v>209</v>
       </c>
       <c r="B182" t="inlineStr">
@@ -4076,7 +4076,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="1" t="n">
+      <c r="A183" t="n">
         <v>223</v>
       </c>
       <c r="B183" t="inlineStr">
@@ -4096,7 +4096,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="1" t="n">
+      <c r="A184" t="n">
         <v>233</v>
       </c>
       <c r="B184" t="inlineStr">
@@ -4116,7 +4116,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="1" t="n">
+      <c r="A185" t="n">
         <v>244</v>
       </c>
       <c r="B185" t="inlineStr">
@@ -4136,7 +4136,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="1" t="n">
+      <c r="A186" t="n">
         <v>247</v>
       </c>
       <c r="B186" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="1" t="n">
+      <c r="A187" t="n">
         <v>248</v>
       </c>
       <c r="B187" t="inlineStr">
@@ -4176,7 +4176,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="1" t="n">
+      <c r="A188" t="n">
         <v>259</v>
       </c>
       <c r="B188" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="1" t="n">
+      <c r="A189" t="n">
         <v>297</v>
       </c>
       <c r="B189" t="inlineStr">

</xml_diff>